<commit_message>
fixed asset schedule issues
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/asset_info.xlsx
+++ b/afar_project/csv_path/excel_files/asset_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FRC\FRC\afar_app\afar_project\csv_path\asset_info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AFAR\afar_project\csv_path\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CE93BC-EAF4-4D81-A705-EC1A38E56AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186C47F0-1984-4F28-B0F1-8BB48AF5DA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Category</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Economic Code</t>
   </si>
   <si>
-    <t>Expected Life(pre)</t>
-  </si>
-  <si>
-    <t>Expected Life(post)</t>
-  </si>
-  <si>
     <t>Depriciation Method</t>
   </si>
   <si>
@@ -124,6 +118,9 @@
   </si>
   <si>
     <t>FL</t>
+  </si>
+  <si>
+    <t>Expected Life</t>
   </si>
 </sst>
 </file>
@@ -441,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="I5" sqref="I5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,273 +457,231 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>4112202</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3">
         <v>4112310</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>4112314</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4112204</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>4112101</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>28</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>